<commit_message>
nodes router and data model
</commit_message>
<xml_diff>
--- a/docs/dataModel.xlsx
+++ b/docs/dataModel.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cambo\Docs\Projects\nodes\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9AA4663F-215E-43A8-BAB7-D8B1862AD32E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4292C3-AF8D-45F7-BC0C-5E88E3B94D55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21585" yWindow="3795" windowWidth="17265" windowHeight="15345" xr2:uid="{DC9B6881-A9E2-4365-A497-0DA9F141341F}"/>
+    <workbookView xWindow="41820" yWindow="1500" windowWidth="23145" windowHeight="16620" xr2:uid="{DC9B6881-A9E2-4365-A497-0DA9F141341F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Table" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -189,36 +189,36 @@
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -558,7 +558,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,64 +568,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="11" t="s">
+      <c r="A4" s="11"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="7" t="s">
+      <c r="A5" s="11"/>
+      <c r="B5" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E5" t="s">
@@ -633,40 +633,40 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="11">
+      <c r="A6" s="11"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="4">
         <v>123</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="7" t="s">
+      <c r="A7" s="11"/>
+      <c r="B7" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="11">
+      <c r="A8" s="12"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="4">
         <v>541</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>